<commit_message>
added e2e tests for journal charges
</commit_message>
<xml_diff>
--- a/tests/data/test_billing_journal.xlsx
+++ b/tests/data/test_billing_journal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertsegal/Source/mpt-api-python-client/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F19B303-E9C2-4042-B2BB-D21F44E322D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB931991-E2AD-DD45-8956-92A2AEEFC33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="620" windowWidth="19200" windowHeight="20980" xr2:uid="{B3AE8077-F886-0E43-9722-6417D1842470}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="20980" xr2:uid="{B3AE8077-F886-0E43-9722-6417D1842470}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>External Reference</t>
   </si>
   <si>
-    <t>ORD-7924-7691-0805</t>
-  </si>
-  <si>
     <t>Vendor Invoice Reference</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Source Value</t>
   </si>
   <si>
-    <t>SUB-5839-4140-9574</t>
-  </si>
-  <si>
     <t>Order Search Criteria</t>
   </si>
   <si>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>COM</t>
+  </si>
+  <si>
+    <t>ORD-2413-8980-9419</t>
+  </si>
+  <si>
+    <t>SUB-0356-5642-8669</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,52 +519,52 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -572,37 +572,37 @@
         <v>1234567890</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
       </c>
       <c r="M2">
         <v>10</v>
@@ -614,13 +614,13 @@
         <v>100</v>
       </c>
       <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>28</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>